<commit_message>
Updated to not break things
</commit_message>
<xml_diff>
--- a/sample_data/DataFile-small.xlsx
+++ b/sample_data/DataFile-small.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\GitHub\resident-scheduler\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{AF4A4F30-2DDE-45D5-85CC-DF978F4EF607}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-443" windowWidth="13680" windowHeight="10500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-443" windowWidth="13680" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>MICU_D</t>
   </si>
@@ -147,84 +148,6 @@
   </si>
   <si>
     <t>Week_26</t>
-  </si>
-  <si>
-    <t>Week_27</t>
-  </si>
-  <si>
-    <t>Week_28</t>
-  </si>
-  <si>
-    <t>Week_29</t>
-  </si>
-  <si>
-    <t>Week_30</t>
-  </si>
-  <si>
-    <t>Week_31</t>
-  </si>
-  <si>
-    <t>Week_32</t>
-  </si>
-  <si>
-    <t>Week_33</t>
-  </si>
-  <si>
-    <t>Week_34</t>
-  </si>
-  <si>
-    <t>Week_35</t>
-  </si>
-  <si>
-    <t>Week_36</t>
-  </si>
-  <si>
-    <t>Week_37</t>
-  </si>
-  <si>
-    <t>Week_38</t>
-  </si>
-  <si>
-    <t>Week_39</t>
-  </si>
-  <si>
-    <t>Week_40</t>
-  </si>
-  <si>
-    <t>Week_41</t>
-  </si>
-  <si>
-    <t>Week_42</t>
-  </si>
-  <si>
-    <t>Week_43</t>
-  </si>
-  <si>
-    <t>Week_44</t>
-  </si>
-  <si>
-    <t>Week_45</t>
-  </si>
-  <si>
-    <t>Week_46</t>
-  </si>
-  <si>
-    <t>Week_47</t>
-  </si>
-  <si>
-    <t>Week_48</t>
-  </si>
-  <si>
-    <t>Week_49</t>
-  </si>
-  <si>
-    <t>Week_50</t>
-  </si>
-  <si>
-    <t>Week_51</t>
-  </si>
-  <si>
-    <t>Week_52</t>
   </si>
   <si>
     <t>Clinic_Group</t>
@@ -311,7 +234,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -706,7 +629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -722,13 +645,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
@@ -740,7 +663,7 @@
       </c>
       <c r="C2" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Purple")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
@@ -752,7 +675,7 @@
       </c>
       <c r="C3" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Yellow")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
@@ -760,11 +683,11 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Blue")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
@@ -772,11 +695,11 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Green")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
@@ -784,11 +707,11 @@
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2">
         <f>COUNTIF(Parameters!$B:$B,"Orange")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -802,10 +725,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
@@ -821,49 +744,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="K1" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="M1" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="N1" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="O1" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.5">
@@ -871,13 +794,13 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -892,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -915,16 +838,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -939,7 +862,7 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -965,13 +888,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -986,7 +909,7 @@
         <v>1000</v>
       </c>
       <c r="I4" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1012,13 +935,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1033,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1059,13 +982,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1080,7 +1003,7 @@
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -1106,13 +1029,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1127,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="I7" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1150,16 +1073,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1174,7 +1097,7 @@
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1203,10 +1126,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1221,7 +1144,7 @@
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1248,11 +1171,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1261,15 +1184,15 @@
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
     <col min="4" max="12" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="55" width="7.8125" bestFit="1" customWidth="1"/>
+    <col min="13" max="29" width="7.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -1352,91 +1275,13 @@
       <c r="AC1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1519,91 +1364,13 @@
       <c r="AC2" s="2">
         <v>5</v>
       </c>
-      <c r="AD2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>6</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>4</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="2">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="AS2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AT2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AU2" s="2">
-        <v>6</v>
-      </c>
-      <c r="AV2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX2" s="2">
-        <v>4</v>
-      </c>
-      <c r="AY2" s="2">
-        <v>-4</v>
-      </c>
-      <c r="AZ2" s="2">
-        <v>-4</v>
-      </c>
-      <c r="BA2" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB2" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -1686,94 +1453,16 @@
       <c r="AC3" s="2">
         <v>0</v>
       </c>
-      <c r="AD3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>6</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>6</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="2">
-        <v>5</v>
-      </c>
-      <c r="AQ3" s="2">
-        <v>5</v>
-      </c>
-      <c r="AR3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX3" s="2">
-        <v>4</v>
-      </c>
-      <c r="AY3" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA3" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.5">
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -1806,630 +1495,852 @@
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="O4" s="2">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="P4" s="2">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="Q4" s="2">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="R4" s="2">
         <v>0</v>
       </c>
       <c r="S4" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="T4" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="U4" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="V4" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="W4" s="2">
         <v>0</v>
       </c>
       <c r="X4" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="Y4" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="Z4" s="2">
+        <v>-3</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>-3</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>-4</v>
+      </c>
+      <c r="W5" s="2">
+        <v>-4</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
         <v>7</v>
       </c>
-      <c r="AB4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="2">
-        <v>6</v>
-      </c>
-      <c r="AS4" s="2">
-        <v>6</v>
-      </c>
-      <c r="AT4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY4" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA4" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB4" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="AB5" s="2">
         <v>7</v>
       </c>
-      <c r="L5" s="2">
-        <v>7</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>-4</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>-4</v>
-      </c>
       <c r="AC5" s="2">
-        <v>-4</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>6</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>6</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>-3</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>-3</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>-3</v>
-      </c>
-      <c r="AI5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="2">
-        <v>5</v>
-      </c>
-      <c r="AO5" s="2">
-        <v>5</v>
-      </c>
-      <c r="AP5" s="2">
-        <v>4</v>
-      </c>
-      <c r="AQ5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA5" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB5" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="AA6" s="2">
         <v>7</v>
       </c>
-      <c r="O6" s="2">
-        <v>7</v>
-      </c>
-      <c r="P6" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>6</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>0</v>
-      </c>
       <c r="AB6" s="2">
         <v>0</v>
       </c>
       <c r="AC6" s="2">
         <v>0</v>
       </c>
-      <c r="AD6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="2">
-        <v>5</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>5</v>
-      </c>
-      <c r="AN6" s="2">
-        <v>4</v>
-      </c>
-      <c r="AO6" s="2">
-        <v>4</v>
-      </c>
-      <c r="AP6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY6" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB6" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.5">
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7</v>
+      </c>
+      <c r="L7" s="2">
+        <v>7</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>0</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>-4</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>-4</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>-3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-3</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2">
+        <v>7</v>
+      </c>
+      <c r="S8" s="2">
+        <v>7</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2">
+        <v>0</v>
+      </c>
+      <c r="W8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="X8" s="2">
+        <v>-4</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>-3</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>-3</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+      <c r="R9" s="2">
+        <v>7</v>
+      </c>
+      <c r="S9" s="2">
+        <v>7</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
+      <c r="V9" s="2">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>7</v>
+      </c>
+      <c r="O10" s="2">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2">
         <v>6</v>
       </c>
-      <c r="N7" s="2">
+      <c r="Q10" s="2">
         <v>6</v>
       </c>
-      <c r="O7" s="2">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2">
-        <v>0</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2">
-        <v>0</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="2">
-        <v>7</v>
-      </c>
-      <c r="AE7" s="2">
-        <v>7</v>
-      </c>
-      <c r="AF7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="2">
-        <v>4</v>
-      </c>
-      <c r="AP7" s="2">
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
+        <v>0</v>
+      </c>
+      <c r="W10" s="2">
+        <v>0</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>6</v>
+      </c>
+      <c r="N11" s="2">
+        <v>6</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.5">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AQ7" s="2">
-        <v>5</v>
-      </c>
-      <c r="AR7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB7" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC7" s="2">
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+      <c r="W13" s="2">
+        <v>0</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2444,24 +2355,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.0625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.9375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.8125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.8125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.0625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.9375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
@@ -2475,7 +2384,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -2487,7 +2396,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
@@ -2556,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -2565,19 +2474,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
@@ -2585,28 +2494,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
@@ -2614,28 +2523,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <v>10</v>
       </c>
-      <c r="F6" s="2">
-        <v>6</v>
-      </c>
-      <c r="G6" s="2">
-        <v>20</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
       <c r="I6" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
@@ -2643,27 +2552,201 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="C7" s="2">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="E7" s="2">
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2">
+        <v>20</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2">
         <v>10</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G11" s="2">
         <v>20</v>
       </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>20</v>
+      </c>
+      <c r="I13" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>